<commit_message>
Building final YA dataset
</commit_message>
<xml_diff>
--- a/1 YA/2 Analyses/1 ANOVAs/YA Output 10_14.xlsx
+++ b/1 YA/2 Analyses/1 ANOVAs/YA Output 10_14.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm.000\Documents\GitHub\Spring-2019-Projects\CVOE\5 Manuscript\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm.000\Documents\GitHub\CVOE-2021\1 YA\2 Analyses\1 ANOVAs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF559639-04C3-4904-AAE4-972E7249D542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE6B654-F52F-4E4C-9144-3A936E7BF07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -998,11 +998,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L88"/>
+  <dimension ref="A1:L98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I88" sqref="I88"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3909,486 +3909,866 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B77">
+        <v>2.0833333333333402E-2</v>
+      </c>
+      <c r="C77">
+        <v>2.1052631578947299E-2</v>
+      </c>
+      <c r="D77">
+        <v>2.0942982456140301E-2</v>
+      </c>
+      <c r="E77">
+        <v>1.6949152542372801E-2</v>
+      </c>
+      <c r="F77">
+        <v>1.75438596491229E-2</v>
+      </c>
+      <c r="G77">
+        <v>1.72413793103449E-2</v>
+      </c>
+      <c r="H77">
         <v>0</v>
       </c>
-      <c r="C77">
-        <v>3.1578947368420998E-2</v>
-      </c>
-      <c r="D77">
-        <v>1.5789473684210499E-2</v>
-      </c>
-      <c r="E77">
-        <v>3.4482758620689599E-2</v>
-      </c>
-      <c r="F77">
-        <v>6.7796610169491595E-2</v>
-      </c>
-      <c r="G77">
-        <v>8.6206896551724102E-2</v>
-      </c>
-      <c r="H77">
-        <v>1.7857142857142901E-2</v>
-      </c>
       <c r="I77">
-        <v>5.2007136485280998E-2</v>
+        <v>-3.3991228070174898E-3</v>
       </c>
       <c r="J77">
-        <v>2.0676691729323801E-3</v>
+        <v>-2.0942982456140301E-2</v>
       </c>
       <c r="K77">
-        <v>-3.3313851548802002E-2</v>
+        <v>-5.9470710675002504E-4</v>
       </c>
       <c r="L77">
-        <v>6.8349753694581197E-2</v>
+        <v>1.72413793103449E-2</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
         <v>1.05263157894737E-2</v>
       </c>
-      <c r="C78">
-        <v>3.1578947368420998E-2</v>
-      </c>
       <c r="D78">
-        <v>2.1052631578947399E-2</v>
+        <v>5.2631578947368602E-3</v>
       </c>
       <c r="E78">
-        <v>5.1724137931034503E-2</v>
+        <v>3.4482758620689599E-2</v>
       </c>
       <c r="F78">
-        <v>3.5714285714285698E-2</v>
+        <v>0</v>
       </c>
       <c r="G78">
-        <v>8.1967213114754106E-2</v>
+        <v>6.7796610169491595E-2</v>
       </c>
       <c r="H78">
-        <v>5.1724137931034503E-2</v>
+        <v>1.75438596491229E-2</v>
       </c>
       <c r="I78">
-        <v>1.4661654135338299E-2</v>
+        <v>-5.2631578947368602E-3</v>
       </c>
       <c r="J78">
-        <v>3.06715063520871E-2</v>
+        <v>1.2280701754386E-2</v>
       </c>
       <c r="K78">
-        <v>1.6009852216748801E-2</v>
+        <v>3.4482758620689599E-2</v>
       </c>
       <c r="L78">
-        <v>3.02430751837196E-2</v>
+        <v>5.0252750520368698E-2</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B79">
-        <v>4.2105263157894798E-2</v>
+        <v>0</v>
       </c>
       <c r="C79">
         <v>3.1578947368420998E-2</v>
       </c>
       <c r="D79">
-        <v>3.6842105263157898E-2</v>
+        <v>1.5789473684210499E-2</v>
       </c>
       <c r="E79">
-        <v>6.8965517241379296E-2</v>
+        <v>3.4482758620689599E-2</v>
       </c>
       <c r="F79">
-        <v>5.1724137931034503E-2</v>
+        <v>6.7796610169491595E-2</v>
       </c>
       <c r="G79">
-        <v>6.6666666666666693E-2</v>
+        <v>8.6206896551724102E-2</v>
       </c>
       <c r="H79">
-        <v>1.6949152542372801E-2</v>
+        <v>1.7857142857142901E-2</v>
       </c>
       <c r="I79">
-        <v>1.4882032667876599E-2</v>
+        <v>5.2007136485280998E-2</v>
       </c>
       <c r="J79">
-        <v>-1.98929527207851E-2</v>
+        <v>2.0676691729323801E-3</v>
       </c>
       <c r="K79">
-        <v>1.72413793103449E-2</v>
+        <v>-3.3313851548802002E-2</v>
       </c>
       <c r="L79">
-        <v>4.9717514124293802E-2</v>
+        <v>6.8349753694581197E-2</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>1.05263157894737E-2</v>
       </c>
       <c r="C80">
-        <v>1.05263157894737E-2</v>
+        <v>3.1578947368420998E-2</v>
       </c>
       <c r="D80">
-        <v>5.2631578947368602E-3</v>
+        <v>2.1052631578947399E-2</v>
       </c>
       <c r="E80">
-        <v>3.4482758620689599E-2</v>
+        <v>5.1724137931034503E-2</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>3.5714285714285698E-2</v>
       </c>
       <c r="G80">
-        <v>1.63934426229508E-2</v>
+        <v>8.1967213114754106E-2</v>
       </c>
       <c r="H80">
-        <v>1.75438596491229E-2</v>
+        <v>5.1724137931034503E-2</v>
       </c>
       <c r="I80">
-        <v>-5.2631578947368602E-3</v>
+        <v>1.4661654135338299E-2</v>
       </c>
       <c r="J80">
-        <v>1.2280701754386E-2</v>
+        <v>3.06715063520871E-2</v>
       </c>
       <c r="K80">
-        <v>3.4482758620689599E-2</v>
+        <v>1.6009852216748801E-2</v>
       </c>
       <c r="L80">
-        <v>-1.15041702617202E-3</v>
+        <v>3.02430751837196E-2</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B81">
-        <v>6.25E-2</v>
+        <v>4.2105263157894798E-2</v>
       </c>
       <c r="C81">
         <v>3.1578947368420998E-2</v>
       </c>
       <c r="D81">
+        <v>3.6842105263157898E-2</v>
+      </c>
+      <c r="E81">
+        <v>6.8965517241379296E-2</v>
+      </c>
+      <c r="F81">
+        <v>5.1724137931034503E-2</v>
+      </c>
+      <c r="G81">
+        <v>6.6666666666666693E-2</v>
+      </c>
+      <c r="H81">
+        <v>1.6949152542372801E-2</v>
+      </c>
+      <c r="I81">
+        <v>1.4882032667876599E-2</v>
+      </c>
+      <c r="J81">
+        <v>-1.98929527207851E-2</v>
+      </c>
+      <c r="K81">
+        <v>1.72413793103449E-2</v>
+      </c>
+      <c r="L81">
+        <v>4.9717514124293802E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>91</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>1.05263157894737E-2</v>
+      </c>
+      <c r="D82">
+        <v>5.2631578947368602E-3</v>
+      </c>
+      <c r="E82">
+        <v>3.4482758620689599E-2</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>1.63934426229508E-2</v>
+      </c>
+      <c r="H82">
+        <v>1.75438596491229E-2</v>
+      </c>
+      <c r="I82">
+        <v>-5.2631578947368602E-3</v>
+      </c>
+      <c r="J82">
+        <v>1.2280701754386E-2</v>
+      </c>
+      <c r="K82">
+        <v>3.4482758620689599E-2</v>
+      </c>
+      <c r="L82">
+        <v>-1.15041702617202E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>92</v>
+      </c>
+      <c r="B83">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C83">
+        <v>3.1578947368420998E-2</v>
+      </c>
+      <c r="D83">
         <v>4.7039473684210499E-2</v>
       </c>
-      <c r="E81">
+      <c r="E83">
         <v>3.3898305084745797E-2</v>
       </c>
-      <c r="F81">
+      <c r="F83">
         <v>1.6666666666666701E-2</v>
       </c>
-      <c r="G81">
+      <c r="G83">
         <v>5.1724137931034503E-2</v>
       </c>
-      <c r="H81">
+      <c r="H83">
         <v>0</v>
       </c>
-      <c r="I81">
+      <c r="I83">
         <v>-3.0372807017543801E-2</v>
       </c>
-      <c r="J81">
+      <c r="J83">
         <v>-4.7039473684210499E-2</v>
       </c>
-      <c r="K81">
+      <c r="K83">
         <v>1.72316384180791E-2</v>
       </c>
-      <c r="L81">
+      <c r="L83">
         <v>5.1724137931034503E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>93</v>
+      </c>
+      <c r="B84">
+        <v>2.0833333333333402E-2</v>
+      </c>
+      <c r="C84">
+        <v>1.05263157894737E-2</v>
+      </c>
+      <c r="D84">
+        <v>1.5679824561403499E-2</v>
+      </c>
+      <c r="E84">
+        <v>5.0847457627118599E-2</v>
+      </c>
+      <c r="F84">
+        <v>3.3333333333333298E-2</v>
+      </c>
+      <c r="G84">
+        <v>0.05</v>
+      </c>
+      <c r="H84">
+        <v>6.8965517241379296E-2</v>
+      </c>
+      <c r="I84">
+        <v>1.76535087719298E-2</v>
+      </c>
+      <c r="J84">
+        <v>5.32856926799758E-2</v>
+      </c>
+      <c r="K84">
+        <v>1.7514124293785301E-2</v>
+      </c>
+      <c r="L84">
+        <v>-1.89655172413793E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>94</v>
+      </c>
+      <c r="B85">
+        <v>2.0833333333333402E-2</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>1.6949152542372801E-2</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <v>6.5324858757061502E-3</v>
+      </c>
+      <c r="J85">
+        <v>-1.0416666666666701E-2</v>
+      </c>
+      <c r="K85">
+        <v>-1.6949152542372801E-2</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>97</v>
+      </c>
+      <c r="B86">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C86">
+        <v>2.1052631578947299E-2</v>
+      </c>
+      <c r="D86">
+        <v>2.61513157894737E-2</v>
+      </c>
+      <c r="E86">
+        <v>3.5087719298245598E-2</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>1.6666666666666701E-2</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86">
+        <v>-2.61513157894737E-2</v>
+      </c>
+      <c r="J86">
+        <v>-2.61513157894737E-2</v>
+      </c>
+      <c r="K86">
+        <v>3.5087719298245598E-2</v>
+      </c>
+      <c r="L86">
+        <v>1.6666666666666701E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>98</v>
+      </c>
+      <c r="B87">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C87">
+        <v>1.05263157894737E-2</v>
+      </c>
+      <c r="D87">
+        <v>2.08881578947369E-2</v>
+      </c>
+      <c r="E87">
+        <v>5.2631578947368501E-2</v>
+      </c>
+      <c r="F87">
+        <v>3.4482758620689599E-2</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>1.75438596491229E-2</v>
+      </c>
+      <c r="I87">
+        <v>1.35946007259528E-2</v>
+      </c>
+      <c r="J87">
+        <v>-3.3442982456139999E-3</v>
+      </c>
+      <c r="K87">
+        <v>1.8148820326678899E-2</v>
+      </c>
+      <c r="L87">
+        <v>-1.75438596491229E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>99</v>
+      </c>
+      <c r="B88">
+        <v>2.1052631578947299E-2</v>
+      </c>
+      <c r="C88">
+        <v>1.05263157894737E-2</v>
+      </c>
+      <c r="D88">
+        <v>1.5789473684210499E-2</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>1.75438596491229E-2</v>
+      </c>
+      <c r="H88">
+        <v>1.75438596491229E-2</v>
+      </c>
+      <c r="I88">
+        <v>-1.5789473684210499E-2</v>
+      </c>
+      <c r="J88">
+        <v>1.7543859649123399E-3</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+      <c r="L88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>100</v>
+      </c>
+      <c r="B89">
+        <v>1.04166666666666E-2</v>
+      </c>
+      <c r="C89">
+        <v>2.1052631578947299E-2</v>
+      </c>
+      <c r="D89">
+        <v>1.5734649122807001E-2</v>
+      </c>
+      <c r="E89">
+        <v>5.2631578947368501E-2</v>
+      </c>
+      <c r="F89">
+        <v>1.6949152542372801E-2</v>
+      </c>
+      <c r="G89">
+        <v>5.0847457627118599E-2</v>
+      </c>
+      <c r="H89">
+        <v>1.6949152542372801E-2</v>
+      </c>
+      <c r="I89">
+        <v>1.2145034195658599E-3</v>
+      </c>
+      <c r="J89">
+        <v>1.2145034195658599E-3</v>
+      </c>
+      <c r="K89">
+        <v>3.5682426404995603E-2</v>
+      </c>
+      <c r="L89">
+        <v>3.3898305084745797E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>101</v>
+      </c>
+      <c r="B90">
+        <v>2.0833333333333402E-2</v>
+      </c>
+      <c r="C90">
+        <v>2.1276595744680899E-2</v>
+      </c>
+      <c r="D90">
+        <v>2.1054964539007098E-2</v>
+      </c>
+      <c r="E90">
+        <v>6.8965517241379296E-2</v>
+      </c>
+      <c r="F90">
+        <v>5.0847457627118599E-2</v>
+      </c>
+      <c r="G90">
+        <v>3.3333333333333298E-2</v>
+      </c>
+      <c r="H90">
+        <v>5.2631578947368501E-2</v>
+      </c>
+      <c r="I90">
+        <v>2.97924930881115E-2</v>
+      </c>
+      <c r="J90">
+        <v>3.1576614408361299E-2</v>
+      </c>
+      <c r="K90">
+        <v>1.81180596142607E-2</v>
+      </c>
+      <c r="L90">
+        <v>-1.9298245614035099E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>102</v>
+      </c>
+      <c r="B91">
+        <v>4.1666666666666602E-2</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="E91">
+        <v>0.15517241379310301</v>
+      </c>
+      <c r="F91">
+        <v>7.0175438596491196E-2</v>
+      </c>
+      <c r="G91">
+        <v>0.1</v>
+      </c>
+      <c r="H91">
+        <v>8.9285714285714302E-2</v>
+      </c>
+      <c r="I91">
+        <v>4.9342105263157902E-2</v>
+      </c>
+      <c r="J91">
+        <v>6.8452380952381001E-2</v>
+      </c>
+      <c r="K91">
+        <v>8.4996975196612201E-2</v>
+      </c>
+      <c r="L91">
+        <v>1.0714285714285701E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B83">
-        <f>AVERAGE(B2:B81)</f>
-        <v>2.7190952813608726E-2</v>
-      </c>
-      <c r="C83">
-        <f t="shared" ref="C83:L83" si="0">AVERAGE(C2:C81)</f>
-        <v>4.4191944819131981E-2</v>
-      </c>
-      <c r="D83">
+      <c r="B93">
+        <f>AVERAGE(B2:B91)</f>
+        <v>2.6602728037047916E-2</v>
+      </c>
+      <c r="C93">
+        <f t="shared" ref="C93:L93" si="0">AVERAGE(C2:C91)</f>
+        <v>4.0687725990777523E-2</v>
+      </c>
+      <c r="D93">
         <f t="shared" si="0"/>
-        <v>3.5691448816370347E-2</v>
-      </c>
-      <c r="E83">
+        <v>3.3645227013912711E-2</v>
+      </c>
+      <c r="E93">
         <f t="shared" si="0"/>
-        <v>6.4485815904252883E-2</v>
-      </c>
-      <c r="F83">
+        <v>6.2507038326198625E-2</v>
+      </c>
+      <c r="F93">
         <f t="shared" si="0"/>
-        <v>3.8281155920176863E-2</v>
-      </c>
-      <c r="G83">
+        <v>3.6697484739173884E-2</v>
+      </c>
+      <c r="G93">
         <f t="shared" si="0"/>
-        <v>5.6022529902103081E-2</v>
-      </c>
-      <c r="H83">
+        <v>5.3724796654714711E-2</v>
+      </c>
+      <c r="H93">
         <f t="shared" si="0"/>
-        <v>3.3063469920725501E-2</v>
-      </c>
-      <c r="I83">
+        <v>3.2506012618024931E-2</v>
+      </c>
+      <c r="I93">
         <f t="shared" si="0"/>
-        <v>2.5897071038065095E-3</v>
-      </c>
-      <c r="J83">
+        <v>3.0522577252611802E-3</v>
+      </c>
+      <c r="J93">
         <f t="shared" si="0"/>
-        <v>-2.6279788956448339E-3</v>
-      </c>
-      <c r="K83">
+        <v>-1.1392143958877678E-3</v>
+      </c>
+      <c r="K93">
         <f t="shared" si="0"/>
-        <v>2.6204659984076017E-2</v>
-      </c>
-      <c r="L83">
+        <v>2.580955358702474E-2</v>
+      </c>
+      <c r="L93">
         <f t="shared" si="0"/>
-        <v>2.295905998137758E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+        <v>2.1218784036689788E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B84">
-        <f>STDEV(B2:B81)</f>
-        <v>2.3212788027946123E-2</v>
-      </c>
-      <c r="C84">
-        <f t="shared" ref="C84:L84" si="1">STDEV(C2:C81)</f>
-        <v>3.9886900504168162E-2</v>
-      </c>
-      <c r="D84">
+      <c r="B94">
+        <f>STDEV(B2:B91)</f>
+        <v>2.2234522923919645E-2</v>
+      </c>
+      <c r="C94">
+        <f t="shared" ref="C94:L94" si="1">STDEV(C2:C91)</f>
+        <v>3.8968701530890791E-2</v>
+      </c>
+      <c r="D94">
         <f t="shared" si="1"/>
-        <v>2.7325971022752974E-2</v>
-      </c>
-      <c r="E84">
+        <v>2.6465015433209459E-2</v>
+      </c>
+      <c r="E94">
         <f t="shared" si="1"/>
-        <v>5.9270505875388201E-2</v>
-      </c>
-      <c r="F84">
+        <v>5.7886582273711504E-2</v>
+      </c>
+      <c r="F94">
         <f t="shared" si="1"/>
-        <v>5.1058879512771257E-2</v>
-      </c>
-      <c r="G84">
+        <v>4.8884012523919829E-2</v>
+      </c>
+      <c r="G94">
         <f t="shared" si="1"/>
-        <v>4.9439717576702805E-2</v>
-      </c>
-      <c r="H84">
+        <v>4.812021723928768E-2</v>
+      </c>
+      <c r="H94">
         <f t="shared" si="1"/>
-        <v>4.561347751385704E-2</v>
-      </c>
-      <c r="I84">
+        <v>4.4143945184077091E-2</v>
+      </c>
+      <c r="I94">
         <f t="shared" si="1"/>
-        <v>4.9402416656251343E-2</v>
-      </c>
-      <c r="J84">
+        <v>4.7088329885901246E-2</v>
+      </c>
+      <c r="J94">
         <f t="shared" si="1"/>
-        <v>4.7825148613895328E-2</v>
-      </c>
-      <c r="K84">
+        <v>4.6331460549629354E-2</v>
+      </c>
+      <c r="K94">
         <f t="shared" si="1"/>
-        <v>4.2365372935131068E-2</v>
-      </c>
-      <c r="L84">
+        <v>4.090875956370648E-2</v>
+      </c>
+      <c r="L94">
         <f t="shared" si="1"/>
-        <v>3.4896403537994912E-2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+        <v>3.4061295641342651E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B85">
-        <f>B84/(SQRT(80))</f>
-        <v>2.5952685988890408E-3</v>
-      </c>
-      <c r="C85">
-        <f t="shared" ref="C85:L85" si="2">C84/(SQRT(80))</f>
-        <v>4.4594910469545317E-3</v>
-      </c>
-      <c r="D85">
+      <c r="B95">
+        <f>B94/(SQRT(80))</f>
+        <v>2.4858952352580853E-3</v>
+      </c>
+      <c r="C95">
+        <f t="shared" ref="C95:L95" si="2">C94/(SQRT(80))</f>
+        <v>4.3568332808985961E-3</v>
+      </c>
+      <c r="D95">
         <f t="shared" si="2"/>
-        <v>3.0551364379032549E-3</v>
-      </c>
-      <c r="E85">
+        <v>2.9588786767118696E-3</v>
+      </c>
+      <c r="E95">
         <f t="shared" si="2"/>
-        <v>6.6266440099084344E-3</v>
-      </c>
-      <c r="F85">
+        <v>6.4719166474576624E-3</v>
+      </c>
+      <c r="F95">
         <f t="shared" si="2"/>
-        <v>5.7085562722763933E-3</v>
-      </c>
-      <c r="G85">
+        <v>5.4653987508217899E-3</v>
+      </c>
+      <c r="G95">
         <f t="shared" si="2"/>
-        <v>5.5275284644949315E-3</v>
-      </c>
-      <c r="H85">
+        <v>5.3800038419552255E-3</v>
+      </c>
+      <c r="H95">
         <f t="shared" si="2"/>
-        <v>5.0997418205571219E-3</v>
-      </c>
-      <c r="I85">
+        <v>4.9354431113310419E-3</v>
+      </c>
+      <c r="I95">
         <f t="shared" si="2"/>
-        <v>5.523358094807293E-3</v>
-      </c>
-      <c r="J85">
+        <v>5.2646353285905048E-3</v>
+      </c>
+      <c r="J95">
         <f t="shared" si="2"/>
-        <v>5.3470141667349893E-3</v>
-      </c>
-      <c r="K85">
+        <v>5.1800147642910499E-3</v>
+      </c>
+      <c r="K95">
         <f t="shared" si="2"/>
-        <v>4.7365926887541427E-3</v>
-      </c>
-      <c r="L85">
+        <v>4.5737383629821165E-3</v>
+      </c>
+      <c r="L95">
         <f t="shared" si="2"/>
-        <v>3.9015365240610391E-3</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+        <v>3.8081686227879729E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B86">
-        <f>B85*1.96</f>
-        <v>5.0867264538225201E-3</v>
-      </c>
-      <c r="C86">
-        <f t="shared" ref="C86:L86" si="3">C85*1.96</f>
-        <v>8.7406024520308816E-3</v>
-      </c>
-      <c r="D86">
+      <c r="B96">
+        <f>B95*1.96</f>
+        <v>4.8723546611058469E-3</v>
+      </c>
+      <c r="C96">
+        <f t="shared" ref="C96:L96" si="3">C95*1.96</f>
+        <v>8.5393932305612482E-3</v>
+      </c>
+      <c r="D96">
         <f t="shared" si="3"/>
-        <v>5.9880674182903795E-3</v>
-      </c>
-      <c r="E86">
+        <v>5.799402206355264E-3</v>
+      </c>
+      <c r="E96">
         <f t="shared" si="3"/>
-        <v>1.2988222259420531E-2</v>
-      </c>
-      <c r="F86">
+        <v>1.2684956629017018E-2</v>
+      </c>
+      <c r="F96">
         <f t="shared" si="3"/>
-        <v>1.1188770293661731E-2</v>
-      </c>
-      <c r="G86">
+        <v>1.0712181551610708E-2</v>
+      </c>
+      <c r="G96">
         <f t="shared" si="3"/>
-        <v>1.0833955790410065E-2</v>
-      </c>
-      <c r="H86">
+        <v>1.0544807530232242E-2</v>
+      </c>
+      <c r="H96">
         <f t="shared" si="3"/>
-        <v>9.9954939682919582E-3</v>
-      </c>
-      <c r="I86">
+        <v>9.6734684982088415E-3</v>
+      </c>
+      <c r="I96">
         <f t="shared" si="3"/>
-        <v>1.0825781865822294E-2</v>
-      </c>
-      <c r="J86">
+        <v>1.0318685244037389E-2</v>
+      </c>
+      <c r="J96">
         <f t="shared" si="3"/>
-        <v>1.0480147766800578E-2</v>
-      </c>
-      <c r="K86">
+        <v>1.0152828938010458E-2</v>
+      </c>
+      <c r="K96">
         <f t="shared" si="3"/>
-        <v>9.2837216699581202E-3</v>
-      </c>
-      <c r="L86">
+        <v>8.9645271914449483E-3</v>
+      </c>
+      <c r="L96">
         <f t="shared" si="3"/>
-        <v>7.6470115871596364E-3</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+        <v>7.4640105006644267E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B87">
-        <f>B83+B86</f>
-        <v>3.2277679267431247E-2</v>
-      </c>
-      <c r="C87">
-        <f t="shared" ref="C87:L87" si="4">C83+C86</f>
-        <v>5.2932547271162866E-2</v>
-      </c>
-      <c r="D87">
+      <c r="B97">
+        <f>B93+B96</f>
+        <v>3.1475082698153765E-2</v>
+      </c>
+      <c r="C97">
+        <f t="shared" ref="C97:L97" si="4">C93+C96</f>
+        <v>4.9227119221338773E-2</v>
+      </c>
+      <c r="D97">
         <f t="shared" si="4"/>
-        <v>4.1679516234660728E-2</v>
-      </c>
-      <c r="E87">
+        <v>3.9444629220267972E-2</v>
+      </c>
+      <c r="E97">
         <f t="shared" si="4"/>
-        <v>7.7474038163673417E-2</v>
-      </c>
-      <c r="F87">
+        <v>7.5191994955215641E-2</v>
+      </c>
+      <c r="F97">
         <f t="shared" si="4"/>
-        <v>4.9469926213838597E-2</v>
-      </c>
-      <c r="G87">
+        <v>4.7409666290784594E-2</v>
+      </c>
+      <c r="G97">
         <f t="shared" si="4"/>
-        <v>6.6856485692513151E-2</v>
-      </c>
-      <c r="H87">
+        <v>6.4269604184946955E-2</v>
+      </c>
+      <c r="H97">
         <f t="shared" si="4"/>
-        <v>4.3058963889017463E-2</v>
-      </c>
-      <c r="I87">
+        <v>4.217948111623377E-2</v>
+      </c>
+      <c r="I97">
         <f t="shared" si="4"/>
-        <v>1.3415488969628804E-2</v>
-      </c>
-      <c r="J87">
+        <v>1.3370942969298569E-2</v>
+      </c>
+      <c r="J97">
         <f t="shared" si="4"/>
-        <v>7.8521688711557444E-3</v>
-      </c>
-      <c r="K87">
+        <v>9.0136145421226901E-3</v>
+      </c>
+      <c r="K97">
         <f t="shared" si="4"/>
-        <v>3.5488381654034139E-2</v>
-      </c>
-      <c r="L87">
+        <v>3.477408077846969E-2</v>
+      </c>
+      <c r="L97">
         <f t="shared" si="4"/>
-        <v>3.0606071568537216E-2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+        <v>2.8682794537354214E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B88">
-        <f>B83-B86</f>
-        <v>2.2104226359786205E-2</v>
-      </c>
-      <c r="C88">
-        <f t="shared" ref="C88:L88" si="5">C83-C86</f>
-        <v>3.5451342367101096E-2</v>
-      </c>
-      <c r="D88">
+      <c r="B98">
+        <f>B93-B96</f>
+        <v>2.173037337594207E-2</v>
+      </c>
+      <c r="C98">
+        <f t="shared" ref="C98:L98" si="5">C93-C96</f>
+        <v>3.2148332760216274E-2</v>
+      </c>
+      <c r="D98">
         <f t="shared" si="5"/>
-        <v>2.9703381398079966E-2</v>
-      </c>
-      <c r="E88">
+        <v>2.7845824807557446E-2</v>
+      </c>
+      <c r="E98">
         <f t="shared" si="5"/>
-        <v>5.1497593644832348E-2</v>
-      </c>
-      <c r="F88">
+        <v>4.9822081697181608E-2</v>
+      </c>
+      <c r="F98">
         <f t="shared" si="5"/>
-        <v>2.7092385626515132E-2</v>
-      </c>
-      <c r="G88">
+        <v>2.5985303187563175E-2</v>
+      </c>
+      <c r="G98">
         <f t="shared" si="5"/>
-        <v>4.5188574111693018E-2</v>
-      </c>
-      <c r="H88">
+        <v>4.3179989124482468E-2</v>
+      </c>
+      <c r="H98">
         <f t="shared" si="5"/>
-        <v>2.3067975952433543E-2</v>
-      </c>
-      <c r="I88">
+        <v>2.2832544119816091E-2</v>
+      </c>
+      <c r="I98">
         <f t="shared" si="5"/>
-        <v>-8.2360747620157833E-3</v>
-      </c>
-      <c r="J88">
+        <v>-7.2664275187762084E-3</v>
+      </c>
+      <c r="J98">
         <f t="shared" si="5"/>
-        <v>-1.3108126662445412E-2</v>
-      </c>
-      <c r="K88">
+        <v>-1.1292043333898227E-2</v>
+      </c>
+      <c r="K98">
         <f t="shared" si="5"/>
-        <v>1.6920938314117895E-2</v>
-      </c>
-      <c r="L88">
+        <v>1.684502639557979E-2</v>
+      </c>
+      <c r="L98">
         <f t="shared" si="5"/>
-        <v>1.5312048394217945E-2</v>
+        <v>1.3754773536025361E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4399,11 +4779,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L88"/>
+  <dimension ref="A1:L98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C83" sqref="C83:L85"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7310,486 +7690,866 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B77">
-        <v>604.59375</v>
+        <v>668.563829787234</v>
       </c>
       <c r="C77">
-        <v>829.01086956521704</v>
+        <v>688.91397849462396</v>
       </c>
       <c r="D77">
-        <v>716.80230978260897</v>
+        <v>678.73890414092898</v>
       </c>
       <c r="E77">
-        <v>1728.75</v>
+        <v>1462.56896551724</v>
       </c>
       <c r="F77">
-        <v>1284.8181818181799</v>
+        <v>1336.30357142857</v>
       </c>
       <c r="G77">
-        <v>1979.03773584906</v>
+        <v>1673.4912280701801</v>
       </c>
       <c r="H77">
-        <v>1430.0909090909099</v>
+        <v>1353.9649122807</v>
       </c>
       <c r="I77">
-        <v>568.01587203557301</v>
+        <v>657.56466728764303</v>
       </c>
       <c r="J77">
-        <v>713.28859930830004</v>
+        <v>675.22600813977294</v>
       </c>
       <c r="K77">
-        <v>443.93181818181802</v>
+        <v>126.26539408867001</v>
       </c>
       <c r="L77">
-        <v>548.94682675814795</v>
+        <v>319.52631578947398</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B78">
-        <v>598.95744680851101</v>
+        <v>610.45833333333303</v>
       </c>
       <c r="C78">
-        <v>671.43478260869597</v>
+        <v>639.01063829787199</v>
       </c>
       <c r="D78">
-        <v>635.19611470860298</v>
+        <v>624.73448581560297</v>
       </c>
       <c r="E78">
-        <v>1351.70909090909</v>
+        <v>1321.0357142857099</v>
       </c>
       <c r="F78">
-        <v>1328.9814814814799</v>
+        <v>1274.1803278688501</v>
       </c>
       <c r="G78">
-        <v>1347.07142857143</v>
+        <v>1174.8727272727299</v>
       </c>
       <c r="H78">
-        <v>1146.72727272727</v>
+        <v>1203.6071428571399</v>
       </c>
       <c r="I78">
-        <v>693.78536677287798</v>
+        <v>649.44584205324998</v>
       </c>
       <c r="J78">
-        <v>511.53115801867</v>
+        <v>578.87265704154004</v>
       </c>
       <c r="K78">
-        <v>22.727609427609401</v>
+        <v>46.855386416861798</v>
       </c>
       <c r="L78">
-        <v>200.34415584415601</v>
+        <v>-28.7344155844157</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B79">
-        <v>587.91208791208805</v>
+        <v>604.59375</v>
       </c>
       <c r="C79">
-        <v>605.18478260869597</v>
+        <v>829.01086956521704</v>
       </c>
       <c r="D79">
-        <v>596.54843526039201</v>
+        <v>716.80230978260897</v>
       </c>
       <c r="E79">
-        <v>1152.75925925926</v>
+        <v>1728.75</v>
       </c>
       <c r="F79">
-        <v>786.76363636363601</v>
+        <v>1284.8181818181799</v>
       </c>
       <c r="G79">
-        <v>1297.82142857143</v>
+        <v>1979.03773584906</v>
       </c>
       <c r="H79">
-        <v>1063.93103448276</v>
+        <v>1430.0909090909099</v>
       </c>
       <c r="I79">
-        <v>190.21520110324499</v>
+        <v>568.01587203557301</v>
       </c>
       <c r="J79">
-        <v>467.38259922236699</v>
+        <v>713.28859930830004</v>
       </c>
       <c r="K79">
-        <v>365.995622895623</v>
+        <v>443.93181818181802</v>
       </c>
       <c r="L79">
-        <v>233.89039408867001</v>
+        <v>548.94682675814795</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B80">
-        <v>472.94791666666703</v>
+        <v>598.95744680851101</v>
       </c>
       <c r="C80">
-        <v>590.67021276595699</v>
+        <v>671.43478260869597</v>
       </c>
       <c r="D80">
-        <v>531.80906471631204</v>
+        <v>635.19611470860298</v>
       </c>
       <c r="E80">
-        <v>1403.5178571428601</v>
+        <v>1351.70909090909</v>
       </c>
       <c r="F80">
-        <v>1321.3220338983101</v>
+        <v>1328.9814814814799</v>
       </c>
       <c r="G80">
-        <v>1234.9666666666701</v>
+        <v>1347.07142857143</v>
       </c>
       <c r="H80">
-        <v>1170.3392857142901</v>
+        <v>1146.72727272727</v>
       </c>
       <c r="I80">
-        <v>789.51296918199296</v>
+        <v>693.78536677287798</v>
       </c>
       <c r="J80">
-        <v>638.53022099797397</v>
+        <v>511.53115801867</v>
       </c>
       <c r="K80">
-        <v>82.195823244552003</v>
+        <v>22.727609427609401</v>
       </c>
       <c r="L80">
-        <v>64.627380952380904</v>
+        <v>200.34415584415601</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81">
+        <v>90</v>
+      </c>
+      <c r="B81">
+        <v>587.91208791208805</v>
+      </c>
+      <c r="C81">
+        <v>605.18478260869597</v>
+      </c>
+      <c r="D81">
+        <v>596.54843526039201</v>
+      </c>
+      <c r="E81">
+        <v>1152.75925925926</v>
+      </c>
+      <c r="F81">
+        <v>786.76363636363601</v>
+      </c>
+      <c r="G81">
+        <v>1297.82142857143</v>
+      </c>
+      <c r="H81">
+        <v>1063.93103448276</v>
+      </c>
+      <c r="I81">
+        <v>190.21520110324499</v>
+      </c>
+      <c r="J81">
+        <v>467.38259922236699</v>
+      </c>
+      <c r="K81">
+        <v>365.995622895623</v>
+      </c>
+      <c r="L81">
+        <v>233.89039408867001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>91</v>
+      </c>
+      <c r="B82">
+        <v>472.94791666666703</v>
+      </c>
+      <c r="C82">
+        <v>590.67021276595699</v>
+      </c>
+      <c r="D82">
+        <v>531.80906471631204</v>
+      </c>
+      <c r="E82">
+        <v>1403.5178571428601</v>
+      </c>
+      <c r="F82">
+        <v>1321.3220338983101</v>
+      </c>
+      <c r="G82">
+        <v>1234.9666666666701</v>
+      </c>
+      <c r="H82">
+        <v>1170.3392857142901</v>
+      </c>
+      <c r="I82">
+        <v>789.51296918199296</v>
+      </c>
+      <c r="J82">
+        <v>638.53022099797397</v>
+      </c>
+      <c r="K82">
+        <v>82.195823244552003</v>
+      </c>
+      <c r="L82">
+        <v>64.627380952380904</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83">
         <v>92</v>
       </c>
-      <c r="B81">
+      <c r="B83">
         <v>521.78888888888901</v>
       </c>
-      <c r="C81">
+      <c r="C83">
         <v>520.35869565217399</v>
       </c>
-      <c r="D81">
+      <c r="D83">
         <v>521.07379227053104</v>
       </c>
-      <c r="E81">
+      <c r="E83">
         <v>1110.7719298245599</v>
       </c>
-      <c r="F81">
+      <c r="F83">
         <v>948.23728813559296</v>
       </c>
-      <c r="G81">
+      <c r="G83">
         <v>1125.03636363636</v>
       </c>
-      <c r="H81">
+      <c r="H83">
         <v>961.79661016949103</v>
       </c>
-      <c r="I81">
+      <c r="I83">
         <v>427.16349586506198</v>
       </c>
-      <c r="J81">
+      <c r="J83">
         <v>440.72281789895999</v>
       </c>
-      <c r="K81">
+      <c r="K83">
         <v>162.53464168896801</v>
       </c>
-      <c r="L81">
+      <c r="L83">
         <v>163.239753466872</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>93</v>
+      </c>
+      <c r="B84">
+        <v>522.659574468085</v>
+      </c>
+      <c r="C84">
+        <v>584.48936170212801</v>
+      </c>
+      <c r="D84">
+        <v>553.57446808510599</v>
+      </c>
+      <c r="E84">
+        <v>1022.07142857143</v>
+      </c>
+      <c r="F84">
+        <v>987.41379310344803</v>
+      </c>
+      <c r="G84">
+        <v>1008.68421052632</v>
+      </c>
+      <c r="H84">
+        <v>1005.33333333333</v>
+      </c>
+      <c r="I84">
+        <v>433.83932501834198</v>
+      </c>
+      <c r="J84">
+        <v>451.75886524822698</v>
+      </c>
+      <c r="K84">
+        <v>34.657635467980299</v>
+      </c>
+      <c r="L84">
+        <v>3.3508771929824701</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>94</v>
+      </c>
+      <c r="B85">
+        <v>891.29787234042601</v>
+      </c>
+      <c r="C85">
+        <v>1024.36263736264</v>
+      </c>
+      <c r="D85">
+        <v>957.83025485153098</v>
+      </c>
+      <c r="E85">
+        <v>1354.44642857143</v>
+      </c>
+      <c r="F85">
+        <v>1500.08620689655</v>
+      </c>
+      <c r="G85">
+        <v>1450.14754098361</v>
+      </c>
+      <c r="H85">
+        <v>1387.12280701754</v>
+      </c>
+      <c r="I85">
+        <v>542.25595204501997</v>
+      </c>
+      <c r="J85">
+        <v>429.292552166012</v>
+      </c>
+      <c r="K85">
+        <v>-145.63977832512299</v>
+      </c>
+      <c r="L85">
+        <v>63.024733966062698</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>97</v>
+      </c>
+      <c r="B86">
+        <v>443.78494623655899</v>
+      </c>
+      <c r="C86">
+        <v>484.64516129032302</v>
+      </c>
+      <c r="D86">
+        <v>464.21505376344101</v>
+      </c>
+      <c r="E86">
+        <v>1173.5818181818199</v>
+      </c>
+      <c r="F86">
+        <v>1220.5084745762699</v>
+      </c>
+      <c r="G86">
+        <v>1262.18644067797</v>
+      </c>
+      <c r="H86">
+        <v>1175.6206896551701</v>
+      </c>
+      <c r="I86">
+        <v>756.29342081283005</v>
+      </c>
+      <c r="J86">
+        <v>711.40563589173098</v>
+      </c>
+      <c r="K86">
+        <v>-46.926656394453197</v>
+      </c>
+      <c r="L86">
+        <v>86.565751022793805</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>98</v>
+      </c>
+      <c r="B87">
+        <v>639.462365591398</v>
+      </c>
+      <c r="C87">
+        <v>620.26595744680901</v>
+      </c>
+      <c r="D87">
+        <v>629.86416151910305</v>
+      </c>
+      <c r="E87">
+        <v>1016.53703703704</v>
+      </c>
+      <c r="F87">
+        <v>916.42857142857099</v>
+      </c>
+      <c r="G87">
+        <v>1149.08771929825</v>
+      </c>
+      <c r="H87">
+        <v>949.625</v>
+      </c>
+      <c r="I87">
+        <v>286.564409909468</v>
+      </c>
+      <c r="J87">
+        <v>319.76083848089701</v>
+      </c>
+      <c r="K87">
+        <v>100.10846560846601</v>
+      </c>
+      <c r="L87">
+        <v>199.46271929824599</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>99</v>
+      </c>
+      <c r="B88">
+        <v>868.04301075268802</v>
+      </c>
+      <c r="C88">
+        <v>874.95744680851101</v>
+      </c>
+      <c r="D88">
+        <v>871.50022878059895</v>
+      </c>
+      <c r="E88">
+        <v>1757.6896551724101</v>
+      </c>
+      <c r="F88">
+        <v>1373.9152542372899</v>
+      </c>
+      <c r="G88">
+        <v>1819</v>
+      </c>
+      <c r="H88">
+        <v>1360.44642857143</v>
+      </c>
+      <c r="I88">
+        <v>502.41502545668902</v>
+      </c>
+      <c r="J88">
+        <v>488.94619979082898</v>
+      </c>
+      <c r="K88">
+        <v>383.77440093512598</v>
+      </c>
+      <c r="L88">
+        <v>458.55357142857099</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>100</v>
+      </c>
+      <c r="B89">
+        <v>531.51578947368398</v>
+      </c>
+      <c r="C89">
+        <v>557.18279569892502</v>
+      </c>
+      <c r="D89">
+        <v>544.34929258630495</v>
+      </c>
+      <c r="E89">
+        <v>1107.7037037037001</v>
+      </c>
+      <c r="F89">
+        <v>1005.25862068966</v>
+      </c>
+      <c r="G89">
+        <v>1267.2678571428601</v>
+      </c>
+      <c r="H89">
+        <v>958.55172413793105</v>
+      </c>
+      <c r="I89">
+        <v>460.90932810335102</v>
+      </c>
+      <c r="J89">
+        <v>414.202431551627</v>
+      </c>
+      <c r="K89">
+        <v>102.445083014049</v>
+      </c>
+      <c r="L89">
+        <v>308.71613300492601</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>101</v>
+      </c>
+      <c r="B90">
+        <v>706.468085106383</v>
+      </c>
+      <c r="C90">
+        <v>895.07608695652198</v>
+      </c>
+      <c r="D90">
+        <v>800.77208603145198</v>
+      </c>
+      <c r="E90">
+        <v>1283.5</v>
+      </c>
+      <c r="F90">
+        <v>1172.42857142857</v>
+      </c>
+      <c r="G90">
+        <v>1221.8620689655199</v>
+      </c>
+      <c r="H90">
+        <v>1201.2777777777801</v>
+      </c>
+      <c r="I90">
+        <v>371.65648539711901</v>
+      </c>
+      <c r="J90">
+        <v>400.50569174632602</v>
+      </c>
+      <c r="K90">
+        <v>111.071428571429</v>
+      </c>
+      <c r="L90">
+        <v>20.584291187739399</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>102</v>
+      </c>
+      <c r="B91">
+        <v>567.01086956521704</v>
+      </c>
+      <c r="C91">
+        <v>605.58947368421002</v>
+      </c>
+      <c r="D91">
+        <v>586.30017162471404</v>
+      </c>
+      <c r="E91">
+        <v>1293.0204081632701</v>
+      </c>
+      <c r="F91">
+        <v>1448.05660377358</v>
+      </c>
+      <c r="G91">
+        <v>1304.25925925926</v>
+      </c>
+      <c r="H91">
+        <v>1360.8235294117601</v>
+      </c>
+      <c r="I91">
+        <v>861.756432148871</v>
+      </c>
+      <c r="J91">
+        <v>774.52335778705105</v>
+      </c>
+      <c r="K91">
+        <v>-155.03619561031999</v>
+      </c>
+      <c r="L91">
+        <v>-56.564270152505301</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B83">
-        <f>AVERAGE(B2:B81)</f>
-        <v>648.4289801458774</v>
-      </c>
-      <c r="C83">
-        <f t="shared" ref="C83:L83" si="0">AVERAGE(C2:C81)</f>
-        <v>712.47990443702201</v>
-      </c>
-      <c r="D83">
+      <c r="B93">
+        <f>AVERAGE(B2:B91)</f>
+        <v>648.03981209250207</v>
+      </c>
+      <c r="C93">
+        <f t="shared" ref="C93:L93" si="0">AVERAGE(C2:C91)</f>
+        <v>710.8098432522703</v>
+      </c>
+      <c r="D93">
         <f t="shared" si="0"/>
-        <v>680.45444229144914</v>
-      </c>
-      <c r="E83">
+        <v>679.42482767238573</v>
+      </c>
+      <c r="E93">
         <f t="shared" si="0"/>
-        <v>1419.4555506342815</v>
-      </c>
-      <c r="F83">
+        <v>1403.8733245549618</v>
+      </c>
+      <c r="F93">
         <f t="shared" si="0"/>
-        <v>1346.9750684401849</v>
-      </c>
-      <c r="G83">
+        <v>1333.2509496738462</v>
+      </c>
+      <c r="G93">
         <f t="shared" si="0"/>
-        <v>1442.9139389411507</v>
-      </c>
-      <c r="H83">
+        <v>1430.7108240832081</v>
+      </c>
+      <c r="H93">
         <f t="shared" si="0"/>
-        <v>1255.0974103709891</v>
-      </c>
-      <c r="I83">
+        <v>1248.4907352746882</v>
+      </c>
+      <c r="I93">
         <f t="shared" si="0"/>
-        <v>666.52062614873546</v>
-      </c>
-      <c r="J83">
+        <v>653.82612200146036</v>
+      </c>
+      <c r="J93">
         <f t="shared" si="0"/>
-        <v>574.64296807953929</v>
-      </c>
-      <c r="K83">
+        <v>569.06590760230188</v>
+      </c>
+      <c r="K93">
         <f t="shared" si="0"/>
-        <v>72.480482194096936</v>
-      </c>
-      <c r="L83">
+        <v>70.622374881116002</v>
+      </c>
+      <c r="L93">
         <f t="shared" si="0"/>
-        <v>187.81652857016186</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+        <v>182.22008880852025</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B84">
-        <f>STDEV(B2:B81)</f>
-        <v>140.00974975619286</v>
-      </c>
-      <c r="C84">
-        <f t="shared" ref="C84:L84" si="1">STDEV(C2:C81)</f>
-        <v>172.64502515374915</v>
-      </c>
-      <c r="D84">
+      <c r="B94">
+        <f>STDEV(B2:B91)</f>
+        <v>139.78749962862523</v>
+      </c>
+      <c r="C94">
+        <f t="shared" ref="C94:L94" si="1">STDEV(C2:C91)</f>
+        <v>171.89452321159172</v>
+      </c>
+      <c r="D94">
         <f t="shared" si="1"/>
-        <v>147.82163320342221</v>
-      </c>
-      <c r="E84">
+        <v>148.01985201458402</v>
+      </c>
+      <c r="E94">
         <f t="shared" si="1"/>
-        <v>304.03121204835861</v>
-      </c>
-      <c r="F84">
+        <v>298.3673701434185</v>
+      </c>
+      <c r="F94">
         <f t="shared" si="1"/>
-        <v>320.97861057676528</v>
-      </c>
-      <c r="G84">
+        <v>311.57243122080035</v>
+      </c>
+      <c r="G94">
         <f t="shared" si="1"/>
-        <v>358.54091761309121</v>
-      </c>
-      <c r="H84">
+        <v>348.59542394104676</v>
+      </c>
+      <c r="H94">
         <f t="shared" si="1"/>
-        <v>290.87927259728792</v>
-      </c>
-      <c r="I84">
+        <v>280.15449410333468</v>
+      </c>
+      <c r="I94">
         <f t="shared" si="1"/>
-        <v>247.31027934290694</v>
-      </c>
-      <c r="J84">
+        <v>242.50500977174872</v>
+      </c>
+      <c r="J94">
         <f t="shared" si="1"/>
-        <v>217.28837872546183</v>
-      </c>
-      <c r="K84">
+        <v>210.95070176486999</v>
+      </c>
+      <c r="K94">
         <f t="shared" si="1"/>
-        <v>165.13124714011818</v>
-      </c>
-      <c r="L84">
+        <v>163.27133177483844</v>
+      </c>
+      <c r="L94">
         <f t="shared" si="1"/>
-        <v>148.64141670425931</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+        <v>151.48931567822899</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B85">
-        <f>B84/(SQRT(80))</f>
-        <v>15.653565898379091</v>
-      </c>
-      <c r="C85">
-        <f t="shared" ref="C85:L85" si="2">C84/(SQRT(80))</f>
-        <v>19.302300611047208</v>
-      </c>
-      <c r="D85">
+      <c r="B95">
+        <f>B94/(SQRT(80))</f>
+        <v>15.62871757871663</v>
+      </c>
+      <c r="C95">
+        <f t="shared" ref="C95:L95" si="2">C94/(SQRT(80))</f>
+        <v>19.218391943051728</v>
+      </c>
+      <c r="D95">
         <f t="shared" si="2"/>
-        <v>16.526961019394601</v>
-      </c>
-      <c r="E85">
+        <v>16.549122556203454</v>
+      </c>
+      <c r="E95">
         <f t="shared" si="2"/>
-        <v>33.991722871089145</v>
-      </c>
-      <c r="F85">
+        <v>33.358486095426244</v>
+      </c>
+      <c r="F95">
         <f t="shared" si="2"/>
-        <v>35.886499628654008</v>
-      </c>
-      <c r="G85">
+        <v>34.834856806229368</v>
+      </c>
+      <c r="G95">
         <f t="shared" si="2"/>
-        <v>40.086093224901177</v>
-      </c>
-      <c r="H85">
+        <v>38.974153228876908</v>
+      </c>
+      <c r="H95">
         <f t="shared" si="2"/>
-        <v>32.521291338661378</v>
-      </c>
-      <c r="I85">
+        <v>31.322224650856015</v>
+      </c>
+      <c r="I95">
         <f t="shared" si="2"/>
-        <v>27.650129807260097</v>
-      </c>
-      <c r="J85">
+        <v>27.112884336694044</v>
+      </c>
+      <c r="J95">
         <f t="shared" si="2"/>
-        <v>24.293579277542587</v>
-      </c>
-      <c r="K85">
+        <v>23.585005452376706</v>
+      </c>
+      <c r="K95">
         <f t="shared" si="2"/>
-        <v>18.462234690731098</v>
-      </c>
-      <c r="L85">
+        <v>18.254289831273006</v>
+      </c>
+      <c r="L95">
         <f t="shared" si="2"/>
-        <v>16.618615601129829</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+        <v>16.937020386072234</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B86">
-        <f>B85*1.96</f>
-        <v>30.680989160823017</v>
-      </c>
-      <c r="C86">
-        <f t="shared" ref="C86:L86" si="3">C85*1.96</f>
-        <v>37.832509197652527</v>
-      </c>
-      <c r="D86">
+      <c r="B96">
+        <f>B95*1.96</f>
+        <v>30.632286454284596</v>
+      </c>
+      <c r="C96">
+        <f t="shared" ref="C96:L96" si="3">C95*1.96</f>
+        <v>37.668048208381386</v>
+      </c>
+      <c r="D96">
         <f t="shared" si="3"/>
-        <v>32.392843598013421</v>
-      </c>
-      <c r="E86">
+        <v>32.43628021015877</v>
+      </c>
+      <c r="E96">
         <f t="shared" si="3"/>
-        <v>66.623776827334723</v>
-      </c>
-      <c r="F86">
+        <v>65.38263274703543</v>
+      </c>
+      <c r="F96">
         <f t="shared" si="3"/>
-        <v>70.337539272161848</v>
-      </c>
-      <c r="G86">
+        <v>68.276319340209554</v>
+      </c>
+      <c r="G96">
         <f t="shared" si="3"/>
-        <v>78.568742720806299</v>
-      </c>
-      <c r="H86">
+        <v>76.389340328598735</v>
+      </c>
+      <c r="H96">
         <f t="shared" si="3"/>
-        <v>63.741731023776296</v>
-      </c>
-      <c r="I86">
+        <v>61.391560315677786</v>
+      </c>
+      <c r="I96">
         <f t="shared" si="3"/>
-        <v>54.19425442222979</v>
-      </c>
-      <c r="J86">
+        <v>53.141253299920329</v>
+      </c>
+      <c r="J96">
         <f t="shared" si="3"/>
-        <v>47.615415383983468</v>
-      </c>
-      <c r="K86">
+        <v>46.22661068665834</v>
+      </c>
+      <c r="K96">
         <f t="shared" si="3"/>
-        <v>36.185979993832952</v>
-      </c>
-      <c r="L86">
+        <v>35.778408069295089</v>
+      </c>
+      <c r="L96">
         <f t="shared" si="3"/>
-        <v>32.572486578214466</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+        <v>33.196559956701577</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B87">
-        <f>B83+B86</f>
-        <v>679.10996930670046</v>
-      </c>
-      <c r="C87">
-        <f t="shared" ref="C87:L87" si="4">C83+C86</f>
-        <v>750.3124136346745</v>
-      </c>
-      <c r="D87">
+      <c r="B97">
+        <f>B93+B96</f>
+        <v>678.67209854678663</v>
+      </c>
+      <c r="C97">
+        <f t="shared" ref="C97:L97" si="4">C93+C96</f>
+        <v>748.47789146065168</v>
+      </c>
+      <c r="D97">
         <f t="shared" si="4"/>
-        <v>712.84728588946257</v>
-      </c>
-      <c r="E87">
+        <v>711.8611078825445</v>
+      </c>
+      <c r="E97">
         <f t="shared" si="4"/>
-        <v>1486.0793274616162</v>
-      </c>
-      <c r="F87">
+        <v>1469.2559573019971</v>
+      </c>
+      <c r="F97">
         <f t="shared" si="4"/>
-        <v>1417.3126077123468</v>
-      </c>
-      <c r="G87">
+        <v>1401.5272690140557</v>
+      </c>
+      <c r="G97">
         <f t="shared" si="4"/>
-        <v>1521.482681661957</v>
-      </c>
-      <c r="H87">
+        <v>1507.1001644118069</v>
+      </c>
+      <c r="H97">
         <f t="shared" si="4"/>
-        <v>1318.8391413947654</v>
-      </c>
-      <c r="I87">
+        <v>1309.8822955903659</v>
+      </c>
+      <c r="I97">
         <f t="shared" si="4"/>
-        <v>720.71488057096531</v>
-      </c>
-      <c r="J87">
+        <v>706.96737530138068</v>
+      </c>
+      <c r="J97">
         <f t="shared" si="4"/>
-        <v>622.2583834635227</v>
-      </c>
-      <c r="K87">
+        <v>615.2925182889602</v>
+      </c>
+      <c r="K97">
         <f t="shared" si="4"/>
-        <v>108.66646218792988</v>
-      </c>
-      <c r="L87">
+        <v>106.4007829504111</v>
+      </c>
+      <c r="L97">
         <f t="shared" si="4"/>
-        <v>220.38901514837633</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+        <v>215.41664876522182</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B88">
-        <f>B83-B86</f>
-        <v>617.74799098505434</v>
-      </c>
-      <c r="C88">
-        <f t="shared" ref="C88:L88" si="5">C83-C86</f>
-        <v>674.64739523936953</v>
-      </c>
-      <c r="D88">
+      <c r="B98">
+        <f>B93-B96</f>
+        <v>617.40752563821752</v>
+      </c>
+      <c r="C98">
+        <f t="shared" ref="C98:L98" si="5">C93-C96</f>
+        <v>673.14179504388892</v>
+      </c>
+      <c r="D98">
         <f t="shared" si="5"/>
-        <v>648.06159869343571</v>
-      </c>
-      <c r="E88">
+        <v>646.98854746222696</v>
+      </c>
+      <c r="E98">
         <f t="shared" si="5"/>
-        <v>1352.8317738069468</v>
-      </c>
-      <c r="F88">
+        <v>1338.4906918079264</v>
+      </c>
+      <c r="F98">
         <f t="shared" si="5"/>
-        <v>1276.6375291680231</v>
-      </c>
-      <c r="G88">
+        <v>1264.9746303336367</v>
+      </c>
+      <c r="G98">
         <f t="shared" si="5"/>
-        <v>1364.3451962203444</v>
-      </c>
-      <c r="H88">
+        <v>1354.3214837546093</v>
+      </c>
+      <c r="H98">
         <f t="shared" si="5"/>
-        <v>1191.3556793472128</v>
-      </c>
-      <c r="I88">
+        <v>1187.0991749590105</v>
+      </c>
+      <c r="I98">
         <f t="shared" si="5"/>
-        <v>612.32637172650561</v>
-      </c>
-      <c r="J88">
+        <v>600.68486870154004</v>
+      </c>
+      <c r="J98">
         <f t="shared" si="5"/>
-        <v>527.02755269555587</v>
-      </c>
-      <c r="K88">
+        <v>522.83929691564356</v>
+      </c>
+      <c r="K98">
         <f t="shared" si="5"/>
-        <v>36.294502200263985</v>
-      </c>
-      <c r="L88">
+        <v>34.843966811820913</v>
+      </c>
+      <c r="L98">
         <f t="shared" si="5"/>
-        <v>155.2440419919474</v>
+        <v>149.02352885181867</v>
       </c>
     </row>
   </sheetData>
@@ -10663,47 +11423,47 @@
         <v>12</v>
       </c>
       <c r="B78">
-        <f>AVERAGE(B1:B76)</f>
+        <f t="shared" ref="B78:L78" si="0">AVERAGE(B1:B76)</f>
         <v>-0.64498199979168269</v>
       </c>
       <c r="C78">
-        <f>AVERAGE(C1:C76)</f>
+        <f t="shared" si="0"/>
         <v>-0.55565747846290203</v>
       </c>
       <c r="D78">
-        <f>AVERAGE(D1:D76)</f>
+        <f t="shared" si="0"/>
         <v>-0.60031973912729231</v>
       </c>
       <c r="E78">
-        <f>AVERAGE(E1:E76)</f>
+        <f t="shared" si="0"/>
         <v>0.43756104540243879</v>
       </c>
       <c r="F78">
-        <f>AVERAGE(F1:F76)</f>
+        <f t="shared" si="0"/>
         <v>0.32129597611633176</v>
       </c>
       <c r="G78">
-        <f>AVERAGE(G1:G76)</f>
+        <f t="shared" si="0"/>
         <v>0.45619230162818208</v>
       </c>
       <c r="H78">
-        <f>AVERAGE(H1:H76)</f>
+        <f t="shared" si="0"/>
         <v>0.19915612866182525</v>
       </c>
       <c r="I78">
-        <f>AVERAGE(I1:I76)</f>
+        <f t="shared" si="0"/>
         <v>0.92161571524362351</v>
       </c>
       <c r="J78">
-        <f>AVERAGE(J1:J76)</f>
+        <f t="shared" si="0"/>
         <v>0.79947586778911772</v>
       </c>
       <c r="K78">
-        <f>AVERAGE(K1:K76)</f>
+        <f t="shared" si="0"/>
         <v>0.11626506928610694</v>
       </c>
       <c r="L78">
-        <f>AVERAGE(L1:L76)</f>
+        <f t="shared" si="0"/>
         <v>0.25703617296635672</v>
       </c>
     </row>
@@ -10712,47 +11472,47 @@
         <v>13</v>
       </c>
       <c r="B79">
-        <f>STDEV(B1:B76)</f>
+        <f t="shared" ref="B79:L79" si="1">STDEV(B1:B76)</f>
         <v>0.14615612118341029</v>
       </c>
       <c r="C79">
-        <f>STDEV(C1:C76)</f>
+        <f t="shared" si="1"/>
         <v>0.15522150065066256</v>
       </c>
       <c r="D79">
-        <f>STDEV(D1:D76)</f>
+        <f t="shared" si="1"/>
         <v>0.13742431556572313</v>
       </c>
       <c r="E79">
-        <f>STDEV(E1:E76)</f>
+        <f t="shared" si="1"/>
         <v>0.19706219192957009</v>
       </c>
       <c r="F79">
-        <f>STDEV(F1:F76)</f>
+        <f t="shared" si="1"/>
         <v>0.22093329045644569</v>
       </c>
       <c r="G79">
-        <f>STDEV(G1:G76)</f>
+        <f t="shared" si="1"/>
         <v>0.23576927211226642</v>
       </c>
       <c r="H79">
-        <f>STDEV(H1:H76)</f>
+        <f t="shared" si="1"/>
         <v>0.1697485109571879</v>
       </c>
       <c r="I79">
-        <f>STDEV(I1:I76)</f>
+        <f t="shared" si="1"/>
         <v>0.31989454401437029</v>
       </c>
       <c r="J79">
-        <f>STDEV(J1:J76)</f>
+        <f t="shared" si="1"/>
         <v>0.27676700681818317</v>
       </c>
       <c r="K79">
-        <f>STDEV(K1:K76)</f>
+        <f t="shared" si="1"/>
         <v>0.21334513429380778</v>
       </c>
       <c r="L79">
-        <f>STDEV(L1:L76)</f>
+        <f t="shared" si="1"/>
         <v>0.19629297496194581</v>
       </c>
     </row>
@@ -10765,43 +11525,43 @@
         <v>1.902790625004951E-2</v>
       </c>
       <c r="C80">
-        <f t="shared" ref="C80:L80" si="0">C79/(SQRT(59))</f>
+        <f t="shared" ref="C80:L80" si="2">C79/(SQRT(59))</f>
         <v>2.0208118130519002E-2</v>
       </c>
       <c r="D80">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.7891121985786577E-2</v>
       </c>
       <c r="E80">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.5655312162804828E-2</v>
       </c>
       <c r="F80">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.8763064483934713E-2</v>
       </c>
       <c r="G80">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.0694544779037495E-2</v>
       </c>
       <c r="H80">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.2099373782132743E-2</v>
       </c>
       <c r="I80">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.1646722313938095E-2</v>
       </c>
       <c r="J80">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.6031995213081522E-2</v>
       </c>
       <c r="K80">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.7775170696768454E-2</v>
       </c>
       <c r="L80">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.5555168643481851E-2</v>
       </c>
     </row>
@@ -10814,43 +11574,43 @@
         <v>3.7294696250097036E-2</v>
       </c>
       <c r="C81">
-        <f t="shared" ref="C81:L81" si="1">C80*1.96</f>
+        <f t="shared" ref="C81:L81" si="3">C80*1.96</f>
         <v>3.9607911535817247E-2</v>
       </c>
       <c r="D81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.5066599092141687E-2</v>
       </c>
       <c r="E81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.0284411839097459E-2</v>
       </c>
       <c r="F81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.6375606388512037E-2</v>
       </c>
       <c r="G81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.0161307766913488E-2</v>
       </c>
       <c r="H81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.3314772612980175E-2</v>
       </c>
       <c r="I81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.1627575735318661E-2</v>
       </c>
       <c r="J81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.0622710617639778E-2</v>
       </c>
       <c r="K81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.4439334565666166E-2</v>
       </c>
       <c r="L81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.0088130541224428E-2</v>
       </c>
     </row>
@@ -10863,43 +11623,43 @@
         <v>-0.60768730354158562</v>
       </c>
       <c r="C82">
-        <f t="shared" ref="C82:L82" si="2">C78+C81</f>
+        <f t="shared" ref="C82:L82" si="4">C78+C81</f>
         <v>-0.51604956692708481</v>
       </c>
       <c r="D82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-0.56525314003515059</v>
       </c>
       <c r="E82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.48784545724153627</v>
       </c>
       <c r="F82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.37767158250484378</v>
       </c>
       <c r="G82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.51635360939509556</v>
       </c>
       <c r="H82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.24247090127480542</v>
       </c>
       <c r="I82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.0032432909789422</v>
       </c>
       <c r="J82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.87009857840675753</v>
       </c>
       <c r="K82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.1707044038517731</v>
       </c>
       <c r="L82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.30712430350758113</v>
       </c>
     </row>
@@ -10912,43 +11672,43 @@
         <v>-0.68227669604177976</v>
       </c>
       <c r="C83">
-        <f t="shared" ref="C83:L83" si="3">C78-C81</f>
+        <f t="shared" ref="C83:L83" si="5">C78-C81</f>
         <v>-0.59526538999871925</v>
       </c>
       <c r="D83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-0.63538633821943402</v>
       </c>
       <c r="E83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.3872766335633413</v>
       </c>
       <c r="F83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26492036972781974</v>
       </c>
       <c r="G83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.39603099386126861</v>
       </c>
       <c r="H83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.15584135604884508</v>
       </c>
       <c r="I83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.83998813950830487</v>
       </c>
       <c r="J83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.72885315717147792</v>
       </c>
       <c r="K83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.1825734720440777E-2</v>
       </c>
       <c r="L83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.20694804242513229</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Starting back on the manuscript
</commit_message>
<xml_diff>
--- a/1 YA/2 Analyses/1 ANOVAs/YA Output 10_14.xlsx
+++ b/1 YA/2 Analyses/1 ANOVAs/YA Output 10_14.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmaxwell\Documents\GitHub\CVOE-2021\1 YA\2 Analyses\1 ANOVAs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm.000\Documents\GitHub\CVOE-2021\1 YA\2 Analyses\1 ANOVAs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065C7037-4B73-4F99-8B7A-2DB0DDFE4CE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B27A2F-9FBD-46D6-AD65-10F7B5A692A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ERRORS" sheetId="1" r:id="rId1"/>
@@ -261,7 +261,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,6 +441,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -602,10 +608,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -963,9 +970,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2806,41 +2813,41 @@
         <v>3.1675465407057499E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="49" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
         <v>57</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="3">
         <v>0.104166666666667</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="3">
         <v>0.12631578947368399</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="3">
         <v>0.11524122807017501</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="3">
         <v>5.2631578947368501E-2</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="3">
         <v>8.3333333333333398E-2</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="3">
         <v>9.8360655737704902E-2</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="3">
         <v>8.77192982456141E-2</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="3">
         <v>-3.1907894736842003E-2</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="3">
         <v>-2.7521929824561302E-2</v>
       </c>
-      <c r="K49">
+      <c r="K49" s="3">
         <v>-3.07017543859649E-2</v>
       </c>
-      <c r="L49">
+      <c r="L49" s="3">
         <v>1.0641357492090799E-2</v>
       </c>
     </row>
@@ -4331,47 +4338,47 @@
         <v>12</v>
       </c>
       <c r="B90">
-        <f>AVERAGE(B2:B88)</f>
+        <f t="shared" ref="B90:L90" si="0">AVERAGE(B2:B88)</f>
         <v>2.6511385294902077E-2</v>
       </c>
       <c r="C90">
-        <f>AVERAGE(C2:C88)</f>
+        <f t="shared" si="0"/>
         <v>3.25581073778154E-2</v>
       </c>
       <c r="D90">
-        <f>AVERAGE(D2:D88)</f>
+        <f t="shared" si="0"/>
         <v>2.9534746336358716E-2</v>
       </c>
       <c r="E90">
-        <f>AVERAGE(E2:E88)</f>
+        <f t="shared" si="0"/>
         <v>6.0259069604152685E-2</v>
       </c>
       <c r="F90">
-        <f>AVERAGE(F2:F88)</f>
+        <f t="shared" si="0"/>
         <v>3.5492198030588271E-2</v>
       </c>
       <c r="G90">
-        <f>AVERAGE(G2:G88)</f>
+        <f t="shared" si="0"/>
         <v>5.5234263651551353E-2</v>
       </c>
       <c r="H90">
-        <f>AVERAGE(H2:H88)</f>
+        <f t="shared" si="0"/>
         <v>3.2868674552675066E-2</v>
       </c>
       <c r="I90">
-        <f>AVERAGE(I2:I88)</f>
+        <f t="shared" si="0"/>
         <v>5.9574516942295661E-3</v>
       </c>
       <c r="J90">
-        <f>AVERAGE(J2:J88)</f>
+        <f t="shared" si="0"/>
         <v>3.333928216316341E-3</v>
       </c>
       <c r="K90">
-        <f>AVERAGE(K2:K88)</f>
+        <f t="shared" si="0"/>
         <v>2.476687157356439E-2</v>
       </c>
       <c r="L90">
-        <f>AVERAGE(L2:L88)</f>
+        <f t="shared" si="0"/>
         <v>2.2365589098876284E-2</v>
       </c>
     </row>
@@ -4380,47 +4387,47 @@
         <v>13</v>
       </c>
       <c r="B91">
-        <f>STDEV(B2:B88)</f>
+        <f t="shared" ref="B91:L91" si="1">STDEV(B2:B88)</f>
         <v>2.3353769939004874E-2</v>
       </c>
       <c r="C91">
-        <f>STDEV(C2:C88)</f>
+        <f t="shared" si="1"/>
         <v>3.1622101996825074E-2</v>
       </c>
       <c r="D91">
-        <f>STDEV(D2:D88)</f>
+        <f t="shared" si="1"/>
         <v>2.4183903534280165E-2</v>
       </c>
       <c r="E91">
-        <f>STDEV(E2:E88)</f>
+        <f t="shared" si="1"/>
         <v>5.6431542904787836E-2</v>
       </c>
       <c r="F91">
-        <f>STDEV(F2:F88)</f>
+        <f t="shared" si="1"/>
         <v>4.7625160156382997E-2</v>
       </c>
       <c r="G91">
-        <f>STDEV(G2:G88)</f>
+        <f t="shared" si="1"/>
         <v>4.8984230306785718E-2</v>
       </c>
       <c r="H91">
-        <f>STDEV(H2:H88)</f>
+        <f t="shared" si="1"/>
         <v>4.4757294808329295E-2</v>
       </c>
       <c r="I91">
-        <f>STDEV(I2:I88)</f>
+        <f t="shared" si="1"/>
         <v>4.7684513583627255E-2</v>
       </c>
       <c r="J91">
-        <f>STDEV(J2:J88)</f>
+        <f t="shared" si="1"/>
         <v>4.5170855798954579E-2</v>
       </c>
       <c r="K91">
-        <f>STDEV(K2:K88)</f>
+        <f t="shared" si="1"/>
         <v>4.0536725597810366E-2</v>
       </c>
       <c r="L91">
-        <f>STDEV(L2:L88)</f>
+        <f t="shared" si="1"/>
         <v>3.3221744488838918E-2</v>
       </c>
     </row>
@@ -4433,43 +4440,43 @@
         <v>2.6110308557253008E-3</v>
       </c>
       <c r="C92">
-        <f t="shared" ref="C92:L92" si="0">C91/(SQRT(80))</f>
+        <f t="shared" ref="C92:L92" si="2">C91/(SQRT(80))</f>
         <v>3.5354584828166352E-3</v>
       </c>
       <c r="D92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.7038426131973932E-3</v>
       </c>
       <c r="E92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.3092383005150772E-3</v>
       </c>
       <c r="F92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.3246547774493443E-3</v>
       </c>
       <c r="G92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.476603439573912E-3</v>
       </c>
       <c r="H92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.0040176840211361E-3</v>
       </c>
       <c r="I92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.3312906923501319E-3</v>
       </c>
       <c r="J92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.0502552084151506E-3</v>
       </c>
       <c r="K92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.5321437010979885E-3</v>
       </c>
       <c r="L92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.7143039504086411E-3</v>
       </c>
     </row>
@@ -4482,43 +4489,43 @@
         <v>5.1176204772215893E-3</v>
       </c>
       <c r="C93">
-        <f t="shared" ref="C93:L93" si="1">C92*1.96</f>
+        <f t="shared" ref="C93:L93" si="3">C92*1.96</f>
         <v>6.9294986263206048E-3</v>
       </c>
       <c r="D93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.2995315218668905E-3</v>
       </c>
       <c r="E93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.2366107069009551E-2</v>
       </c>
       <c r="F93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0436323363800714E-2</v>
       </c>
       <c r="G93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0734142741564867E-2</v>
       </c>
       <c r="H93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.8078746606814274E-3</v>
       </c>
       <c r="I93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0449329757006258E-2</v>
       </c>
       <c r="J93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.8985002084936956E-3</v>
       </c>
       <c r="K93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.8830016541520569E-3</v>
       </c>
       <c r="L93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.280035742800936E-3</v>
       </c>
     </row>
@@ -4531,43 +4538,43 @@
         <v>3.1629005772123665E-2</v>
       </c>
       <c r="C94">
-        <f t="shared" ref="C94:L94" si="2">C90+C93</f>
+        <f t="shared" ref="C94:L94" si="4">C90+C93</f>
         <v>3.9487606004136006E-2</v>
       </c>
       <c r="D94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.4834277858225605E-2</v>
       </c>
       <c r="E94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.2625176673162234E-2</v>
       </c>
       <c r="F94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.5928521394388987E-2</v>
       </c>
       <c r="G94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.5968406393116213E-2</v>
       </c>
       <c r="H94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.2676549213356493E-2</v>
       </c>
       <c r="I94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.6406781451235825E-2</v>
       </c>
       <c r="J94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.3232428424810037E-2</v>
       </c>
       <c r="K94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.3649873227716447E-2</v>
       </c>
       <c r="L94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.964562484167722E-2</v>
       </c>
     </row>
@@ -4580,43 +4587,43 @@
         <v>2.1393764817680488E-2</v>
       </c>
       <c r="C95">
-        <f t="shared" ref="C95:L95" si="3">C90-C93</f>
+        <f t="shared" ref="C95:L95" si="5">C90-C93</f>
         <v>2.5628608751494794E-2</v>
       </c>
       <c r="D95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.4235214814491826E-2</v>
       </c>
       <c r="E95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.7892962535143135E-2</v>
       </c>
       <c r="F95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.5055874666787555E-2</v>
       </c>
       <c r="G95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.4500120909986486E-2</v>
       </c>
       <c r="H95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.3060799891993639E-2</v>
       </c>
       <c r="I95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-4.4918780627766922E-3</v>
       </c>
       <c r="J95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-6.5645719921773541E-3</v>
       </c>
       <c r="K95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.5883869919412333E-2</v>
       </c>
       <c r="L95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.5085553356075348E-2</v>
       </c>
     </row>
@@ -4630,9 +4637,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6473,41 +6480,41 @@
         <v>232.45614035087701</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="49" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
         <v>57</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="3">
         <v>417.25581395348797</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="3">
         <v>562.65060240963896</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="3">
         <v>489.95320818156301</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="3">
         <v>992.72222222222194</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="3">
         <v>845.05454545454495</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="3">
         <v>913.327272727273</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="3">
         <v>867.288461538462</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="3">
         <v>355.10133727298199</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="3">
         <v>377.33525335689802</v>
       </c>
-      <c r="K49">
+      <c r="K49" s="3">
         <v>147.66767676767699</v>
       </c>
-      <c r="L49">
+      <c r="L49" s="3">
         <v>46.038811188811202</v>
       </c>
     </row>
@@ -7998,47 +8005,47 @@
         <v>12</v>
       </c>
       <c r="B90">
-        <f>AVERAGE(B2:B88)</f>
+        <f t="shared" ref="B90:L90" si="0">AVERAGE(B2:B88)</f>
         <v>635.22952775412637</v>
       </c>
       <c r="C90">
-        <f>AVERAGE(C2:C88)</f>
+        <f t="shared" si="0"/>
         <v>706.28465117548058</v>
       </c>
       <c r="D90">
-        <f>AVERAGE(D2:D88)</f>
+        <f t="shared" si="0"/>
         <v>670.75708946480302</v>
       </c>
       <c r="E90">
-        <f>AVERAGE(E2:E88)</f>
+        <f t="shared" si="0"/>
         <v>1407.6774261581318</v>
       </c>
       <c r="F90">
-        <f>AVERAGE(F2:F88)</f>
+        <f t="shared" si="0"/>
         <v>1316.8144125848148</v>
       </c>
       <c r="G90">
-        <f>AVERAGE(G2:G88)</f>
+        <f t="shared" si="0"/>
         <v>1431.731230866304</v>
       </c>
       <c r="H90">
-        <f>AVERAGE(H2:H88)</f>
+        <f t="shared" si="0"/>
         <v>1242.7551207654251</v>
       </c>
       <c r="I90">
-        <f>AVERAGE(I2:I88)</f>
+        <f t="shared" si="0"/>
         <v>646.05732312001203</v>
       </c>
       <c r="J90">
-        <f>AVERAGE(J2:J88)</f>
+        <f t="shared" si="0"/>
         <v>571.99803130062151</v>
       </c>
       <c r="K90">
-        <f>AVERAGE(K2:K88)</f>
+        <f t="shared" si="0"/>
         <v>90.86301357331655</v>
       </c>
       <c r="L90">
-        <f>AVERAGE(L2:L88)</f>
+        <f t="shared" si="0"/>
         <v>188.97611010087908</v>
       </c>
     </row>
@@ -8047,47 +8054,47 @@
         <v>13</v>
       </c>
       <c r="B91">
-        <f>STDEV(B2:B88)</f>
+        <f t="shared" ref="B91:L91" si="1">STDEV(B2:B88)</f>
         <v>131.23489638003937</v>
       </c>
       <c r="C91">
-        <f>STDEV(C2:C88)</f>
+        <f t="shared" si="1"/>
         <v>185.32084086978651</v>
       </c>
       <c r="D91">
-        <f>STDEV(D2:D88)</f>
+        <f t="shared" si="1"/>
         <v>150.0072670653575</v>
       </c>
       <c r="E91">
-        <f>STDEV(E2:E88)</f>
+        <f t="shared" si="1"/>
         <v>345.77497021170581</v>
       </c>
       <c r="F91">
-        <f>STDEV(F2:F88)</f>
+        <f t="shared" si="1"/>
         <v>361.3776527974253</v>
       </c>
       <c r="G91">
-        <f>STDEV(G2:G88)</f>
+        <f t="shared" si="1"/>
         <v>420.41075422565137</v>
       </c>
       <c r="H91">
-        <f>STDEV(H2:H88)</f>
+        <f t="shared" si="1"/>
         <v>336.87174719526564</v>
       </c>
       <c r="I91">
-        <f>STDEV(I2:I88)</f>
+        <f t="shared" si="1"/>
         <v>276.16655140210037</v>
       </c>
       <c r="J91">
-        <f>STDEV(J2:J88)</f>
+        <f t="shared" si="1"/>
         <v>247.2616102738171</v>
       </c>
       <c r="K91">
-        <f>STDEV(K2:K88)</f>
+        <f t="shared" si="1"/>
         <v>170.37317981451875</v>
       </c>
       <c r="L91">
-        <f>STDEV(L2:L88)</f>
+        <f t="shared" si="1"/>
         <v>154.91182604714908</v>
       </c>
     </row>
@@ -8100,43 +8107,43 @@
         <v>14.672507466295455</v>
       </c>
       <c r="C92">
-        <f t="shared" ref="C92:L92" si="0">C91/(SQRT(80))</f>
+        <f t="shared" ref="C92:L92" si="2">C91/(SQRT(80))</f>
         <v>20.719499891613193</v>
       </c>
       <c r="D92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16.771322313855237</v>
       </c>
       <c r="E92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>38.658816915566952</v>
       </c>
       <c r="F92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>40.403249860217997</v>
       </c>
       <c r="G92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>47.003351246025666</v>
       </c>
       <c r="H92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>37.663406321386901</v>
       </c>
       <c r="I92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>30.876359102339311</v>
       </c>
       <c r="J92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>27.644688439915768</v>
       </c>
       <c r="K92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>19.048300580402945</v>
       </c>
       <c r="L92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>17.319668678002394</v>
       </c>
     </row>
@@ -8149,43 +8156,43 @@
         <v>28.758114633939091</v>
       </c>
       <c r="C93">
-        <f t="shared" ref="C93:L93" si="1">C92*1.96</f>
+        <f t="shared" ref="C93:L93" si="3">C92*1.96</f>
         <v>40.61021978756186</v>
       </c>
       <c r="D93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>32.871791735156265</v>
       </c>
       <c r="E93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>75.771281154511229</v>
       </c>
       <c r="F93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>79.190369726027271</v>
       </c>
       <c r="G93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>92.126568442210299</v>
       </c>
       <c r="H93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>73.82027638991832</v>
       </c>
       <c r="I93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>60.517663840585051</v>
       </c>
       <c r="J93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>54.183589342234903</v>
       </c>
       <c r="K93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>37.334669137589771</v>
       </c>
       <c r="L93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>33.946550608884692</v>
       </c>
     </row>
@@ -8198,43 +8205,43 @@
         <v>663.98764238806541</v>
       </c>
       <c r="C94">
-        <f t="shared" ref="C94:L94" si="2">C90+C93</f>
+        <f t="shared" ref="C94:L94" si="4">C90+C93</f>
         <v>746.89487096304242</v>
       </c>
       <c r="D94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>703.62888119995932</v>
       </c>
       <c r="E94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1483.4487073126429</v>
       </c>
       <c r="F94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1396.0047823108421</v>
       </c>
       <c r="G94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1523.8577993085144</v>
       </c>
       <c r="H94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1316.5753971553434</v>
       </c>
       <c r="I94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>706.57498696059713</v>
       </c>
       <c r="J94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>626.18162064285639</v>
       </c>
       <c r="K94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>128.19768271090632</v>
       </c>
       <c r="L94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>222.92266070976376</v>
       </c>
     </row>
@@ -8247,43 +8254,43 @@
         <v>606.47141312018732</v>
       </c>
       <c r="C95">
-        <f t="shared" ref="C95:L95" si="3">C90-C93</f>
+        <f t="shared" ref="C95:L95" si="5">C90-C93</f>
         <v>665.67443138791873</v>
       </c>
       <c r="D95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>637.88529772964671</v>
       </c>
       <c r="E95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1331.9061450036206</v>
       </c>
       <c r="F95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1237.6240428587876</v>
       </c>
       <c r="G95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1339.6046624240937</v>
       </c>
       <c r="H95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1168.9348443755068</v>
       </c>
       <c r="I95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>585.53965927942693</v>
       </c>
       <c r="J95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>517.81444195838662</v>
       </c>
       <c r="K95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>53.52834443572678</v>
       </c>
       <c r="L95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>155.02955949199441</v>
       </c>
     </row>

</xml_diff>